<commit_message>
Fixing test data for test Test_11_CartPageMainOperation.
</commit_message>
<xml_diff>
--- a/Luma/tests/Test_11_CartPageMainOperation.xlsx
+++ b/Luma/tests/Test_11_CartPageMainOperation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git-project\luma-repo\Luma\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5D2895-46EF-4C27-92E7-F3B3C4E0AC60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E7F741-4D33-444A-A1B9-21F602D63959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29340" yWindow="1305" windowWidth="28275" windowHeight="10590" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProductPage_1" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>data_id</t>
   </si>
@@ -79,12 +79,6 @@
     <t>M</t>
   </si>
   <si>
-    <t>29.0</t>
-  </si>
-  <si>
-    <t>34.0</t>
-  </si>
-  <si>
     <t>subtotal</t>
   </si>
   <si>
@@ -94,13 +88,13 @@
     <t>238.00</t>
   </si>
   <si>
-    <t>29.000</t>
-  </si>
-  <si>
-    <t>34.000</t>
-  </si>
-  <si>
     <t>qty</t>
+  </si>
+  <si>
+    <t>29.00</t>
+  </si>
+  <si>
+    <t>34.00</t>
   </si>
 </sst>
 </file>
@@ -436,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36589AC9-DEC5-4883-9C60-48FF053B7C55}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,7 +482,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -517,7 +511,7 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -551,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{346E4937-24AA-49B1-9FA7-E9BCD1F12858}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,10 +572,10 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
         <v>14</v>
@@ -601,10 +595,10 @@
         <v>7</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G2">
         <v>5</v>
@@ -627,10 +621,10 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G3">
         <v>7</v>

</xml_diff>